<commit_message>
Start on Iteration 2
+added new menu for semesters
+needs to be further implemented
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Gradebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>User Story</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>As a user, I can delete the current user and start over from scratch.</t>
+  </si>
+  <si>
+    <t>As a student, I will be able to add a semester to my course history</t>
+  </si>
+  <si>
+    <t>As a user, I will be able to add classes to each semester</t>
+  </si>
+  <si>
+    <t>As a user, I will be able to add all necessary course information and final grades to calculate overall GPA</t>
+  </si>
+  <si>
+    <t>As a user, I will have the ability to add grades for each class and specify the weight</t>
+  </si>
+  <si>
+    <t>As a student, I will be able to predict my final grade based on potential grades I input and change based on different outcomes.</t>
   </si>
 </sst>
 </file>
@@ -65,7 +80,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +101,69 @@
       <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,7 +175,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -114,20 +185,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -410,279 +491,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="28.75" customWidth="1"/>
     <col min="2" max="2" width="21.25" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" ht="34.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="3">
         <v>43146</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="3">
         <v>43147</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="3">
         <v>43148</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="3">
         <v>43149</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.25">
-      <c r="A3" s="3"/>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25">
-      <c r="A4" s="3"/>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.25">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="14.25">
-      <c r="A7" s="3" t="s">
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.25">
-      <c r="A8" s="3"/>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25">
-      <c r="A9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.25">
-      <c r="A10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.25">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.25">
-      <c r="A12" s="3" t="s">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.25">
-      <c r="A13" s="3"/>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.25">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.25">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="14.25">
-      <c r="A17" s="3" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.25">
-      <c r="A18" s="3"/>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.25">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="14.25">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="14.25">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="14.25">
-      <c r="A22" s="3" t="s">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="14.25">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="14.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="14.25">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="14.25">
-      <c r="A26" s="3"/>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="39" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>43154</v>
+      </c>
+      <c r="D27" s="7">
+        <v>43157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2"/>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2"/>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="1">
+        <v>15</v>
+      </c>
+      <c r="D39" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2"/>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2"/>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2"/>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A48"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A16"/>
@@ -690,6 +967,7 @@
     <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Removed Old Code and Added More to Semesters
+rough finish of semesters menu
+added funtion to add semesters
+changed menu inputs
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Gradebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
@@ -209,11 +209,11 @@
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
-    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Heading" xfId="1"/>
+    <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -777,6 +777,9 @@
       <c r="E27" s="6">
         <v>43160</v>
       </c>
+      <c r="F27" s="6">
+        <v>43167</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
@@ -794,6 +797,9 @@
       <c r="E28" s="1">
         <v>10</v>
       </c>
+      <c r="F28" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7"/>
@@ -809,6 +815,9 @@
       <c r="E29" s="1">
         <v>3</v>
       </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7"/>
@@ -819,10 +828,10 @@
     <row r="32" spans="1:6">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -838,8 +847,11 @@
       <c r="E34" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="7"/>
       <c r="B35" t="s">
         <v>4</v>
@@ -853,17 +865,20 @@
       <c r="E35" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -879,8 +894,11 @@
       <c r="E39" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="7"/>
       <c r="B40" t="s">
         <v>4</v>
@@ -894,17 +912,20 @@
       <c r="E40" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:6">
       <c r="A43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:6">
       <c r="A44" s="7" t="s">
         <v>14</v>
       </c>
@@ -920,8 +941,11 @@
       <c r="E44" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="7"/>
       <c r="B45" t="s">
         <v>4</v>
@@ -935,17 +959,20 @@
       <c r="E45" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:6">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:6">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:6">
       <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
@@ -961,8 +988,11 @@
       <c r="E49" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>4</v>
@@ -976,28 +1006,31 @@
       <c r="E50" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:6">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:6">
       <c r="A53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A48"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A44:A48"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Further additions to section and assignment classes
+early framework or GPA calculation
+rough final design for system outline
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\Gradebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Desktop\Gradebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD9F2CA-EF92-4624-9850-34F161EE4131}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
@@ -210,11 +209,11 @@
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
-    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Heading" xfId="1"/>
+    <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -491,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -841,18 +840,22 @@
     <row r="30" spans="1:8">
       <c r="A30" s="7"/>
       <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="7"/>
       <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="7"/>
       <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="7"/>
       <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="7" t="s">
@@ -877,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -901,20 +904,23 @@
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="7"/>
       <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="7"/>
       <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="7"/>
       <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7" t="s">
@@ -939,7 +945,7 @@
         <v>13</v>
       </c>
       <c r="H39" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -963,20 +969,23 @@
         <v>5</v>
       </c>
       <c r="H40" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="7"/>
       <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="7"/>
       <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="7"/>
       <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="7" t="s">
@@ -1001,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="H44" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1025,20 +1034,23 @@
         <v>5</v>
       </c>
       <c r="H45" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="7"/>
       <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="7"/>
       <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="7"/>
       <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="7" t="s">
@@ -1063,7 +1075,7 @@
         <v>15</v>
       </c>
       <c r="H49" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1087,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="H50" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:8">

</xml_diff>

<commit_message>
Final Iteration 2 Update, added GPA Functionality
+finished GPA functionality
+polished system interaction
+full implementation of Iteration 2 user stories
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -491,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -682,7 +682,7 @@
     <row r="16" spans="1:6">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
@@ -702,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>7</v>
@@ -720,16 +720,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
@@ -749,19 +749,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="39" customHeight="1">
+    <row r="27" spans="1:9" ht="39" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>0</v>
       </c>
@@ -786,8 +786,11 @@
       <c r="H27" s="6">
         <v>43178</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" s="6">
+        <v>43178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="7" t="s">
         <v>11</v>
       </c>
@@ -812,8 +815,11 @@
       <c r="H28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>4</v>
@@ -836,28 +842,35 @@
       <c r="H29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="7"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="7"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="7"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="7"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -882,8 +895,11 @@
       <c r="H34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="7"/>
       <c r="B35" t="s">
         <v>4</v>
@@ -906,23 +922,29 @@
       <c r="H35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="7"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="7"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="7"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="7" t="s">
         <v>13</v>
       </c>
@@ -947,8 +969,11 @@
       <c r="H39" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="7"/>
       <c r="B40" t="s">
         <v>4</v>
@@ -971,23 +996,29 @@
       <c r="H40" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="7"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="7"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="7"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="7" t="s">
         <v>14</v>
       </c>
@@ -1012,8 +1043,11 @@
       <c r="H44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="7"/>
       <c r="B45" t="s">
         <v>4</v>
@@ -1036,23 +1070,29 @@
       <c r="H45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="7"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="7"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="7"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="7" t="s">
         <v>15</v>
       </c>
@@ -1077,8 +1117,11 @@
       <c r="H49" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="7"/>
       <c r="B50" t="s">
         <v>4</v>
@@ -1101,28 +1144,31 @@
       <c r="H50" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="A49:A53"/>
     <mergeCell ref="A28:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added gui functionality to Major menu
+user can now look at progress and major in
scrollable view
+foundation for create user set up, comments added in createuser file for possible implementation
+restructured user profile
+changed changemajor to createnewuser
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>User Story</t>
   </si>
@@ -83,7 +83,10 @@
     <t>Restructure code</t>
   </si>
   <si>
-    <t>As a user, I can navigate the user profile menu to check my major, progress, change my major, and go to my semesters menu</t>
+    <t>As a user, I can navigate the user profile menu to go to my major menu, and go to my semesters menu</t>
+  </si>
+  <si>
+    <t>As a user, I can navigate the major menu to see my major, progress, and change my major</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -196,17 +199,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -214,9 +214,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -566,887 +570,937 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62:F63"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5"/>
     <col min="2" max="2" width="22"/>
-    <col min="3" max="3" width="11.25" style="3"/>
-    <col min="4" max="4" width="9.75" style="3"/>
-    <col min="5" max="5" width="11.375" style="3"/>
-    <col min="6" max="6" width="10.375" style="3"/>
+    <col min="3" max="3" width="11.25" style="2"/>
+    <col min="4" max="4" width="9.75" style="2"/>
+    <col min="5" max="5" width="11.375" style="2"/>
+    <col min="6" max="6" width="10.375" style="2"/>
     <col min="7" max="1025" width="8.875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="4">
         <v>43146</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <v>43147</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="4">
         <v>43148</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="4">
         <v>43149</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="D2" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="9"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="9"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>8</v>
       </c>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="9"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3">
-        <v>3</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
         <v>2</v>
       </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="9"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="9"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="9"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
     </row>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="9"/>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>2</v>
       </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="9"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+      <c r="A20" s="9"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+      <c r="A21" s="9"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="3">
-        <v>3</v>
-      </c>
-      <c r="D22" s="3">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
         <v>2</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+      <c r="A23" s="9"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+      <c r="A24" s="9"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
+      <c r="A25" s="9"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
+      <c r="A26" s="9"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
     <row r="27" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>43154</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>43157</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>43160</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>43167</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>43177</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <v>43178</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>43178</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>12</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>11</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>10</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>2</v>
       </c>
-      <c r="G28" s="3">
-        <v>0</v>
-      </c>
-      <c r="H28" s="3">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+      <c r="A29" s="9"/>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>4</v>
       </c>
-      <c r="D29" s="3">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="D29" s="2">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="2">
         <v>1</v>
       </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="3">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3">
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+      <c r="A30" s="9"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="9"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="9"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="9"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3">
-        <v>15</v>
-      </c>
-      <c r="D34" s="3">
-        <v>15</v>
-      </c>
-      <c r="E34" s="3">
-        <v>15</v>
-      </c>
-      <c r="F34" s="3">
-        <v>15</v>
-      </c>
-      <c r="G34" s="3">
-        <v>3</v>
-      </c>
-      <c r="H34" s="3">
-        <v>0</v>
-      </c>
-      <c r="I34" s="3">
+      <c r="C34" s="2">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2">
+        <v>15</v>
+      </c>
+      <c r="F34" s="2">
+        <v>15</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="9"/>
       <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="3">
-        <v>5</v>
-      </c>
-      <c r="D35" s="3">
-        <v>5</v>
-      </c>
-      <c r="E35" s="3">
-        <v>5</v>
-      </c>
-      <c r="F35" s="3">
-        <v>5</v>
-      </c>
-      <c r="G35" s="3">
+      <c r="C35" s="2">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5</v>
+      </c>
+      <c r="F35" s="2">
+        <v>5</v>
+      </c>
+      <c r="G35" s="2">
         <v>1</v>
       </c>
-      <c r="H35" s="3">
-        <v>0</v>
-      </c>
-      <c r="I35" s="3">
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+      <c r="A36" s="9"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
+      <c r="A37" s="9"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
+      <c r="A38" s="9"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="3">
-        <v>15</v>
-      </c>
-      <c r="D39" s="3">
-        <v>15</v>
-      </c>
-      <c r="E39" s="3">
-        <v>15</v>
-      </c>
-      <c r="F39" s="3">
-        <v>15</v>
-      </c>
-      <c r="G39" s="3">
+      <c r="C39" s="2">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2">
+        <v>15</v>
+      </c>
+      <c r="F39" s="2">
+        <v>15</v>
+      </c>
+      <c r="G39" s="2">
         <v>13</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>8</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
+      <c r="A40" s="9"/>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="3">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3">
-        <v>5</v>
-      </c>
-      <c r="E40" s="3">
-        <v>5</v>
-      </c>
-      <c r="F40" s="3">
-        <v>5</v>
-      </c>
-      <c r="G40" s="3">
-        <v>5</v>
-      </c>
-      <c r="H40" s="3">
-        <v>3</v>
-      </c>
-      <c r="I40" s="3">
+      <c r="C40" s="2">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2">
+        <v>5</v>
+      </c>
+      <c r="F40" s="2">
+        <v>5</v>
+      </c>
+      <c r="G40" s="2">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2">
+        <v>3</v>
+      </c>
+      <c r="I40" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A41" s="9"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" s="9"/>
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
+      <c r="A43" s="9"/>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="3">
-        <v>15</v>
-      </c>
-      <c r="D44" s="3">
-        <v>15</v>
-      </c>
-      <c r="E44" s="3">
-        <v>15</v>
-      </c>
-      <c r="F44" s="3">
-        <v>15</v>
-      </c>
-      <c r="G44" s="3">
+      <c r="C44" s="2">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2">
+        <v>15</v>
+      </c>
+      <c r="E44" s="2">
+        <v>15</v>
+      </c>
+      <c r="F44" s="2">
+        <v>15</v>
+      </c>
+      <c r="G44" s="2">
         <v>10</v>
       </c>
-      <c r="H44" s="3">
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
+      <c r="A45" s="9"/>
       <c r="B45" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="3">
-        <v>5</v>
-      </c>
-      <c r="D45" s="3">
-        <v>5</v>
-      </c>
-      <c r="E45" s="3">
-        <v>5</v>
-      </c>
-      <c r="F45" s="3">
-        <v>5</v>
-      </c>
-      <c r="G45" s="3">
-        <v>5</v>
-      </c>
-      <c r="H45" s="3">
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="C45" s="2">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>5</v>
+      </c>
+      <c r="E45" s="2">
+        <v>5</v>
+      </c>
+      <c r="F45" s="2">
+        <v>5</v>
+      </c>
+      <c r="G45" s="2">
+        <v>5</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
+      <c r="A46" s="9"/>
       <c r="C46"/>
       <c r="D46"/>
       <c r="E46"/>
       <c r="F46"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
+      <c r="A47" s="9"/>
       <c r="C47"/>
       <c r="D47"/>
       <c r="E47"/>
       <c r="F47"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
+      <c r="A48" s="9"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="3">
-        <v>15</v>
-      </c>
-      <c r="D49" s="3">
-        <v>15</v>
-      </c>
-      <c r="E49" s="3">
-        <v>15</v>
-      </c>
-      <c r="F49" s="3">
-        <v>15</v>
-      </c>
-      <c r="G49" s="3">
-        <v>15</v>
-      </c>
-      <c r="H49" s="3">
+      <c r="C49" s="2">
+        <v>15</v>
+      </c>
+      <c r="D49" s="2">
+        <v>15</v>
+      </c>
+      <c r="E49" s="2">
+        <v>15</v>
+      </c>
+      <c r="F49" s="2">
+        <v>15</v>
+      </c>
+      <c r="G49" s="2">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2">
         <v>11</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
+      <c r="A50" s="9"/>
       <c r="B50" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="3">
-        <v>5</v>
-      </c>
-      <c r="D50" s="3">
-        <v>5</v>
-      </c>
-      <c r="E50" s="3">
-        <v>5</v>
-      </c>
-      <c r="F50" s="3">
-        <v>5</v>
-      </c>
-      <c r="G50" s="3">
-        <v>5</v>
-      </c>
-      <c r="H50" s="3">
+      <c r="C50" s="2">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2">
+        <v>5</v>
+      </c>
+      <c r="E50" s="2">
+        <v>5</v>
+      </c>
+      <c r="F50" s="2">
+        <v>5</v>
+      </c>
+      <c r="G50" s="2">
+        <v>5</v>
+      </c>
+      <c r="H50" s="2">
         <v>4</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+      <c r="A51" s="9"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+      <c r="A52" s="9"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+      <c r="A53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A54" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="8" t="s">
+      <c r="A54" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="8">
         <v>43179</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="8">
         <v>43182</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="8">
         <v>43187</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B55" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <v>10</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="2">
         <v>2</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
+      <c r="A56" s="9"/>
       <c r="B56" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="3">
-        <v>5</v>
-      </c>
-      <c r="D56" s="3">
+      <c r="C56" s="2">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2">
         <v>2</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
+      <c r="A57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
+      <c r="A58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
+      <c r="A59" s="10"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B60" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <v>10</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>10</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
+      <c r="A61" s="9"/>
       <c r="B61" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="3">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3">
-        <v>5</v>
-      </c>
-      <c r="E61" s="3">
+      <c r="C61" s="2">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>5</v>
+      </c>
+      <c r="E61" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
+      <c r="A62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
+      <c r="A63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="A64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="2">
+        <v>10</v>
+      </c>
+      <c r="D65" s="2">
+        <v>10</v>
+      </c>
+      <c r="E65" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="9"/>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="2">
+        <v>5</v>
+      </c>
+      <c r="D66" s="2">
+        <v>5</v>
+      </c>
+      <c r="E66" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="10"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="10"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="10"/>
+      <c r="B69" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="A55:A59"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="A28:A33"/>
@@ -1454,11 +1508,6 @@
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>